<commit_message>
@aashishm27: code update3 forr tetst
</commit_message>
<xml_diff>
--- a/src/main/resources/phone_verification-request.xlsx
+++ b/src/main/resources/phone_verification-request.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\phone-verification-api-mine\src\main\resources\api\request\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amahajan/AnypointStudio/new version/phone-identity-api/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CFACC7-09D5-45DB-AEC3-22622CDA054B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14333A94-C58E-CD4B-8B40-8864F3049CD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,13 +118,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +136,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -151,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,13 +169,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -486,18 +490,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="27.125" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,15 +548,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2">
-        <v>9814097161</v>
+      <c r="C2" s="5">
+        <v>3236603473</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -567,15 +571,15 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2">
-        <v>4807389277</v>
+      <c r="C3" s="5">
+        <v>6264423732</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -590,15 +594,15 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4">
-        <v>0</v>
+      <c r="C4" s="5">
+        <v>5628600011</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -613,7 +617,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -621,7 +625,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="5">
-        <v>510907500013</v>
+        <v>8182078943</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -636,15 +640,15 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2">
-        <v>98140971612</v>
+      <c r="C6" s="5">
+        <v>7148133678</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -659,7 +663,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -667,7 +671,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="5">
-        <v>480738927712</v>
+        <v>5629268836</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -682,14 +686,16 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="5">
+        <v>6263557097</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -703,15 +709,15 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2">
-        <v>51090750000</v>
+      <c r="C9" s="5">
+        <v>6262822724</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -726,7 +732,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -734,7 +740,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="5">
-        <v>510907500013</v>
+        <v>8189528851</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -749,15 +755,15 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="5">
-        <v>1245678901</v>
+        <v>2136255939</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -772,15 +778,15 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="5">
-        <v>6462675079</v>
+        <v>6265182366</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -795,15 +801,15 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="5">
-        <v>4807389277</v>
+        <v>6266887610</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -817,6 +823,206 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C14" s="5">
+        <v>3233528900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C15" s="5">
+        <v>6263500737</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C16" s="5">
+        <v>3232252123</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="5">
+        <v>4157561586</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="5">
+        <v>6266958989</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="5">
+        <v>5624071383</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C20" s="5">
+        <v>3232566816</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C21" s="5">
+        <v>3232229338</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C22" s="5">
+        <v>9093966868</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C23" s="5">
+        <v>6509179682</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C24" s="5">
+        <v>6262801444</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="5">
+        <v>3237210739</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C26" s="5">
+        <v>9094728123</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="5">
+        <v>3232225984</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="5">
+        <v>4014479338</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="5">
+        <v>6266767927</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="5">
+        <v>5625956697</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C31" s="5">
+        <v>3232579667</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C32" s="5">
+        <v>5628601801</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="5">
+        <v>6268076768</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="5">
+        <v>6266176388</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="5">
+        <v>6263080531</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="5">
+        <v>3232440350</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="5">
+        <v>9098607956</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="5">
+        <v>7143238000</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="5">
+        <v>3233639775</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="5">
+        <v>6269614592</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="5">
+        <v>6268209869</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="5">
+        <v>3237226285</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="5">
+        <v>5622566625</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C45" s="5">
+        <v>5037470180</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="5">
+        <v>5624020577</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C48" s="5">
+        <v>6265739416</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="5">
+        <v>7075520654</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="5">
+        <v>4157314234</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="5">
+        <v>4154419770</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52" s="5">
+        <v>6503034621</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53" s="5">
+        <v>4156729547</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>